<commit_message>
Added Cuotas de Uso forecast
</commit_message>
<xml_diff>
--- a/PDN/data.xlsx
+++ b/PDN/data.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexisalvarez\OneDrive - Grupo Vidanta\UPDATE\Work\01. 26Dic18 - Metas PowerBI\Enero2019\_Forecast\GoalsForecastsAndProbabilites\PDN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_3E03D13649EED85128EDDE1AEE2358AA12E1CD1A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{25443DF9-2860-4C2D-A21A-DD88CAA78241}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_3E03D13649EED85128EDDE1AEE2358AA12E1CD1A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4BEBE96C-661E-44C1-866B-44CD20AF6C7B}"/>
   <bookViews>
-    <workbookView xWindow="3996" yWindow="0" windowWidth="18816" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="0" windowWidth="18816" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Año</t>
   </si>
@@ -46,15 +51,71 @@
   </si>
   <si>
     <t>febrero</t>
+  </si>
+  <si>
+    <t>01/02/2019</t>
+  </si>
+  <si>
+    <t>02/02/2019</t>
+  </si>
+  <si>
+    <t>03/02/2019</t>
+  </si>
+  <si>
+    <t>04/02/2019</t>
+  </si>
+  <si>
+    <t>05/02/2019</t>
+  </si>
+  <si>
+    <t>06/02/2019</t>
+  </si>
+  <si>
+    <t>07/02/2019</t>
+  </si>
+  <si>
+    <t>08/02/2019</t>
+  </si>
+  <si>
+    <t>09/02/2019</t>
+  </si>
+  <si>
+    <t>10/02/2019</t>
+  </si>
+  <si>
+    <t>11/02/2019</t>
+  </si>
+  <si>
+    <t>12/02/2019</t>
+  </si>
+  <si>
+    <t>13/02/2019</t>
+  </si>
+  <si>
+    <t>14/02/2019</t>
+  </si>
+  <si>
+    <t>15/02/2019</t>
+  </si>
+  <si>
+    <t>16/02/2019</t>
+  </si>
+  <si>
+    <t>17/02/2019</t>
+  </si>
+  <si>
+    <t>18/02/2019</t>
+  </si>
+  <si>
+    <t>19/02/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy"/>
-    <numFmt numFmtId="165" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -85,18 +146,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -110,14 +182,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F20">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mes"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fechaa"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Producción"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="#Reservas"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="I.P.P.R."/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Producción" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="#Reservas" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="I.P.P.R." dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -420,11 +492,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -455,17 +525,17 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>43497</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="3">
         <v>414254</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="5">
-        <v>41425</v>
+      <c r="F2" s="3">
+        <v>41425.4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -475,16 +545,16 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>43498</v>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="3">
         <v>67365</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>13473</v>
       </c>
     </row>
@@ -495,16 +565,16 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
-        <v>43499</v>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="3">
         <v>10400</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>10400</v>
       </c>
     </row>
@@ -515,16 +585,16 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
-        <v>43500</v>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="3">
         <v>2000</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -535,17 +605,17 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2">
-        <v>43501</v>
+      <c r="C6" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="3">
         <v>81356</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
-        <v>10170</v>
+      <c r="F6" s="3">
+        <v>10169.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -555,17 +625,17 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
-        <v>43502</v>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <v>129179</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>9</v>
       </c>
-      <c r="F7" s="5">
-        <v>14353</v>
+      <c r="F7" s="3">
+        <v>14353.222222222201</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -575,17 +645,17 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
-        <v>43503</v>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="3">
         <v>113575</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>8</v>
       </c>
-      <c r="F8" s="5">
-        <v>14197</v>
+      <c r="F8" s="3">
+        <v>14196.875</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -595,17 +665,17 @@
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>43504</v>
+      <c r="C9" t="s">
+        <v>14</v>
       </c>
       <c r="D9" s="3">
         <v>222214</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>13</v>
       </c>
-      <c r="F9" s="5">
-        <v>17093</v>
+      <c r="F9" s="3">
+        <v>17093.384615384599</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -615,17 +685,17 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
-        <v>43505</v>
+      <c r="C10" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="3">
         <v>77193</v>
       </c>
-      <c r="E10" s="4">
-        <v>6</v>
-      </c>
-      <c r="F10" s="5">
-        <v>12866</v>
+      <c r="E10" s="2">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3">
+        <v>12865.5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -635,16 +705,16 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2">
-        <v>43506</v>
+      <c r="C11" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="3">
         <v>34396</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>34396</v>
       </c>
     </row>
@@ -655,16 +725,16 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2">
-        <v>43507</v>
+      <c r="C12" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="3">
         <v>96536</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>8</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>12067</v>
       </c>
     </row>
@@ -675,17 +745,17 @@
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2">
-        <v>43508</v>
+      <c r="C13" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="3">
         <v>234247</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>15</v>
       </c>
-      <c r="F13" s="5">
-        <v>15616</v>
+      <c r="F13" s="3">
+        <v>15616.4666666667</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -695,17 +765,17 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2">
-        <v>43509</v>
+      <c r="C14" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="3">
         <v>84265</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>7</v>
       </c>
-      <c r="F14" s="5">
-        <v>12038</v>
+      <c r="F14" s="3">
+        <v>12037.857142857099</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -715,17 +785,17 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2">
-        <v>43510</v>
+      <c r="C15" t="s">
+        <v>20</v>
       </c>
       <c r="D15" s="3">
         <v>215446</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>15</v>
       </c>
-      <c r="F15" s="5">
-        <v>14363</v>
+      <c r="F15" s="3">
+        <v>14363.0666666667</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -735,17 +805,17 @@
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
-        <v>43511</v>
+      <c r="C16" t="s">
+        <v>21</v>
       </c>
       <c r="D16" s="3">
         <v>261167</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>20</v>
       </c>
-      <c r="F16" s="5">
-        <v>13058</v>
+      <c r="F16" s="3">
+        <v>13058.35</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -755,17 +825,17 @@
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2">
-        <v>43512</v>
+      <c r="C17" t="s">
+        <v>22</v>
       </c>
       <c r="D17" s="3">
         <v>69495</v>
       </c>
-      <c r="E17" s="4">
-        <v>6</v>
-      </c>
-      <c r="F17" s="5">
-        <v>11583</v>
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3">
+        <v>11582.5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -775,17 +845,17 @@
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="2">
-        <v>43513</v>
+      <c r="C18" t="s">
+        <v>23</v>
       </c>
       <c r="D18" s="3">
         <v>78074</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>4</v>
       </c>
-      <c r="F18" s="5">
-        <v>19519</v>
+      <c r="F18" s="3">
+        <v>19518.5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -795,17 +865,37 @@
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="2">
-        <v>43514</v>
+      <c r="C19" t="s">
+        <v>24</v>
       </c>
       <c r="D19" s="3">
-        <v>49017</v>
-      </c>
-      <c r="E19" s="4">
-        <v>5</v>
-      </c>
-      <c r="F19" s="5">
-        <v>9803</v>
+        <v>97146</v>
+      </c>
+      <c r="E19" s="2">
+        <v>11</v>
+      </c>
+      <c r="F19" s="3">
+        <v>8831.4545454545496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3">
+        <v>86572</v>
+      </c>
+      <c r="E20" s="2">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3">
+        <v>9619.1111111111095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All forecast but Occupancy done. All is left is the probability measure
</commit_message>
<xml_diff>
--- a/PDN/data.xlsx
+++ b/PDN/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexisalvarez\OneDrive - Grupo Vidanta\UPDATE\Work\01. 26Dic18 - Metas PowerBI\Enero2019\_Forecast\GoalsForecastsAndProbabilites\PDN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_3E03D13649EED85128EDDE1AEE2358AA12E1CD1A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4BEBE96C-661E-44C1-866B-44CD20AF6C7B}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="11_3E03D13649EED85128EDDE1AEE2358AA12E1CD1A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E6CC1BE9-A336-4C46-AB69-4B7D0929F7D0}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="0" windowWidth="18816" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9348" yWindow="0" windowWidth="18816" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
   <si>
     <t>Año</t>
   </si>
@@ -51,63 +51,6 @@
   </si>
   <si>
     <t>febrero</t>
-  </si>
-  <si>
-    <t>01/02/2019</t>
-  </si>
-  <si>
-    <t>02/02/2019</t>
-  </si>
-  <si>
-    <t>03/02/2019</t>
-  </si>
-  <si>
-    <t>04/02/2019</t>
-  </si>
-  <si>
-    <t>05/02/2019</t>
-  </si>
-  <si>
-    <t>06/02/2019</t>
-  </si>
-  <si>
-    <t>07/02/2019</t>
-  </si>
-  <si>
-    <t>08/02/2019</t>
-  </si>
-  <si>
-    <t>09/02/2019</t>
-  </si>
-  <si>
-    <t>10/02/2019</t>
-  </si>
-  <si>
-    <t>11/02/2019</t>
-  </si>
-  <si>
-    <t>12/02/2019</t>
-  </si>
-  <si>
-    <t>13/02/2019</t>
-  </si>
-  <si>
-    <t>14/02/2019</t>
-  </si>
-  <si>
-    <t>15/02/2019</t>
-  </si>
-  <si>
-    <t>16/02/2019</t>
-  </si>
-  <si>
-    <t>17/02/2019</t>
-  </si>
-  <si>
-    <t>18/02/2019</t>
-  </si>
-  <si>
-    <t>19/02/2019</t>
   </si>
 </sst>
 </file>
@@ -146,11 +89,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,7 +130,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F27">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mes"/>
@@ -492,11 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -525,17 +478,17 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="C2" s="4">
+        <v>43497</v>
       </c>
       <c r="D2" s="3">
-        <v>414254</v>
+        <v>408255</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>41425.4</v>
+        <v>45362</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -545,8 +498,8 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="C3" s="4">
+        <v>43498</v>
       </c>
       <c r="D3" s="3">
         <v>67365</v>
@@ -565,8 +518,8 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
+      <c r="C4" s="4">
+        <v>43499</v>
       </c>
       <c r="D4" s="3">
         <v>10400</v>
@@ -585,8 +538,8 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
+      <c r="C5" s="4">
+        <v>43500</v>
       </c>
       <c r="D5" s="3">
         <v>2000</v>
@@ -605,8 +558,8 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
+      <c r="C6" s="4">
+        <v>43501</v>
       </c>
       <c r="D6" s="3">
         <v>81356</v>
@@ -615,7 +568,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="3">
-        <v>10169.5</v>
+        <v>10170</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -625,8 +578,8 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="C7" s="4">
+        <v>43502</v>
       </c>
       <c r="D7" s="3">
         <v>129179</v>
@@ -635,7 +588,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>14353.222222222201</v>
+        <v>14353</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -645,8 +598,8 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
+      <c r="C8" s="4">
+        <v>43503</v>
       </c>
       <c r="D8" s="3">
         <v>113575</v>
@@ -655,7 +608,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="3">
-        <v>14196.875</v>
+        <v>14197</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -665,17 +618,17 @@
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
+      <c r="C9" s="4">
+        <v>43504</v>
       </c>
       <c r="D9" s="3">
-        <v>222214</v>
+        <v>207215</v>
       </c>
       <c r="E9" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3">
-        <v>17093.384615384599</v>
+        <v>17268</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -685,8 +638,8 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>15</v>
+      <c r="C10" s="4">
+        <v>43505</v>
       </c>
       <c r="D10" s="3">
         <v>77193</v>
@@ -695,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="3">
-        <v>12865.5</v>
+        <v>12866</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -705,8 +658,8 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
-        <v>16</v>
+      <c r="C11" s="4">
+        <v>43506</v>
       </c>
       <c r="D11" s="3">
         <v>34396</v>
@@ -725,8 +678,8 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
+      <c r="C12" s="4">
+        <v>43507</v>
       </c>
       <c r="D12" s="3">
         <v>96536</v>
@@ -745,8 +698,8 @@
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
+      <c r="C13" s="4">
+        <v>43508</v>
       </c>
       <c r="D13" s="3">
         <v>234247</v>
@@ -755,7 +708,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="3">
-        <v>15616.4666666667</v>
+        <v>15616</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -765,17 +718,17 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
+      <c r="C14" s="4">
+        <v>43509</v>
       </c>
       <c r="D14" s="3">
-        <v>84265</v>
+        <v>78866</v>
       </c>
       <c r="E14" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" s="3">
-        <v>12037.857142857099</v>
+        <v>13144</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -785,8 +738,8 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
-        <v>20</v>
+      <c r="C15" s="4">
+        <v>43510</v>
       </c>
       <c r="D15" s="3">
         <v>215446</v>
@@ -795,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="3">
-        <v>14363.0666666667</v>
+        <v>14363</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -805,8 +758,8 @@
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
-        <v>21</v>
+      <c r="C16" s="4">
+        <v>43511</v>
       </c>
       <c r="D16" s="3">
         <v>261167</v>
@@ -815,7 +768,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="3">
-        <v>13058.35</v>
+        <v>13058</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -825,8 +778,8 @@
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
-        <v>22</v>
+      <c r="C17" s="4">
+        <v>43512</v>
       </c>
       <c r="D17" s="3">
         <v>69495</v>
@@ -835,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="3">
-        <v>11582.5</v>
+        <v>11583</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -845,8 +798,8 @@
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
-        <v>23</v>
+      <c r="C18" s="4">
+        <v>43513</v>
       </c>
       <c r="D18" s="3">
         <v>78074</v>
@@ -855,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="3">
-        <v>19518.5</v>
+        <v>19519</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -865,17 +818,17 @@
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>24</v>
+      <c r="C19" s="4">
+        <v>43514</v>
       </c>
       <c r="D19" s="3">
-        <v>97146</v>
+        <v>93626</v>
       </c>
       <c r="E19" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3">
-        <v>8831.4545454545496</v>
+        <v>9363</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -885,17 +838,157 @@
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
-        <v>25</v>
+      <c r="C20" s="4">
+        <v>43515</v>
       </c>
       <c r="D20" s="3">
-        <v>86572</v>
+        <v>213224</v>
       </c>
       <c r="E20" s="2">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3">
+        <v>13327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4">
+        <v>43516</v>
+      </c>
+      <c r="D21" s="3">
+        <v>153105</v>
+      </c>
+      <c r="E21" s="2">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3">
+        <v>9569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4">
+        <v>43517</v>
+      </c>
+      <c r="D22" s="3">
+        <v>168489</v>
+      </c>
+      <c r="E22" s="2">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3">
+        <v>9911</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4">
+        <v>43518</v>
+      </c>
+      <c r="D23" s="3">
+        <v>134792</v>
+      </c>
+      <c r="E23" s="2">
+        <v>13</v>
+      </c>
+      <c r="F23" s="3">
+        <v>10369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="4">
+        <v>43519</v>
+      </c>
+      <c r="D24" s="3">
+        <v>108725</v>
+      </c>
+      <c r="E24" s="2">
         <v>9</v>
       </c>
-      <c r="F20" s="3">
-        <v>9619.1111111111095</v>
+      <c r="F24" s="3">
+        <v>12081</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="4">
+        <v>43520</v>
+      </c>
+      <c r="D25" s="3">
+        <v>58396</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>14599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4">
+        <v>43521</v>
+      </c>
+      <c r="D26" s="3">
+        <v>327179</v>
+      </c>
+      <c r="E26" s="2">
+        <v>24</v>
+      </c>
+      <c r="F26" s="3">
+        <v>13632</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="4">
+        <v>43522</v>
+      </c>
+      <c r="D27" s="7">
+        <v>210000</v>
+      </c>
+      <c r="E27" s="8">
+        <v>17</v>
+      </c>
+      <c r="F27" s="7">
+        <v>12352.9411764706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scores to forecasts models
</commit_message>
<xml_diff>
--- a/PDN/data.xlsx
+++ b/PDN/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexisalvarez\OneDrive - Grupo Vidanta\UPDATE\Work\01. 26Dic18 - Metas PowerBI\Enero2019\_Forecast\GoalsForecastsAndProbabilites\PDN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_3E03D13649EED85128EDDE1AEE2358AA12E1CD1A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E6CC1BE9-A336-4C46-AB69-4B7D0929F7D0}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="6_{74FE8280-A592-4FC4-BF0E-F114E96E327C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5D35CFE9-BC32-4677-B4B4-59A549289810}"/>
   <bookViews>
-    <workbookView xWindow="9348" yWindow="0" windowWidth="18816" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="0" windowWidth="9030" windowHeight="2480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>Año</t>
   </si>
@@ -50,7 +50,7 @@
     <t>I.P.P.R.</t>
   </si>
   <si>
-    <t>febrero</t>
+    <t>marzo</t>
   </si>
 </sst>
 </file>
@@ -89,21 +89,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
     </dxf>
@@ -112,6 +108,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -130,11 +129,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F14">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fechaa"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fechaa" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Producción" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="#Reservas" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="I.P.P.R." dataDxfId="0"/>
@@ -440,18 +439,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2019</v>
       </c>
@@ -479,19 +478,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="4">
-        <v>43497</v>
+        <v>43525</v>
       </c>
       <c r="D2" s="3">
-        <v>408255</v>
+        <v>204889</v>
       </c>
       <c r="E2" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>45362</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
@@ -499,19 +498,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="4">
-        <v>43498</v>
+        <v>43526</v>
       </c>
       <c r="D3" s="3">
-        <v>67365</v>
+        <v>34996</v>
       </c>
       <c r="E3" s="2">
         <v>5</v>
       </c>
       <c r="F3" s="3">
-        <v>13473</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2019</v>
       </c>
@@ -519,19 +518,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="4">
-        <v>43499</v>
+        <v>43527</v>
       </c>
       <c r="D4" s="3">
-        <v>10400</v>
+        <v>51399</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3">
-        <v>10400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2019</v>
       </c>
@@ -539,19 +538,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="4">
-        <v>43500</v>
+        <v>43528</v>
       </c>
       <c r="D5" s="3">
-        <v>2000</v>
+        <v>252847</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2019</v>
       </c>
@@ -559,19 +558,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="4">
-        <v>43501</v>
+        <v>43529</v>
       </c>
       <c r="D6" s="3">
-        <v>81356</v>
+        <v>304511</v>
       </c>
       <c r="E6" s="2">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3">
-        <v>10170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2019</v>
       </c>
@@ -579,19 +578,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="4">
-        <v>43502</v>
+        <v>43530</v>
       </c>
       <c r="D7" s="3">
-        <v>129179</v>
+        <v>283817</v>
       </c>
       <c r="E7" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3">
-        <v>14353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>18921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2019</v>
       </c>
@@ -599,19 +598,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="4">
-        <v>43503</v>
+        <v>43531</v>
       </c>
       <c r="D8" s="3">
-        <v>113575</v>
+        <v>167152</v>
       </c>
       <c r="E8" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F8" s="3">
-        <v>14197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12858</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2019</v>
       </c>
@@ -619,19 +618,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="4">
-        <v>43504</v>
+        <v>43532</v>
       </c>
       <c r="D9" s="3">
-        <v>207215</v>
+        <v>445397</v>
       </c>
       <c r="E9" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3">
-        <v>17268</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>29693</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2019</v>
       </c>
@@ -639,19 +638,19 @@
         <v>6</v>
       </c>
       <c r="C10" s="4">
-        <v>43505</v>
+        <v>43533</v>
       </c>
       <c r="D10" s="3">
-        <v>77193</v>
+        <v>259888</v>
       </c>
       <c r="E10" s="2">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3">
-        <v>12866</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2019</v>
       </c>
@@ -659,19 +658,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="4">
-        <v>43506</v>
+        <v>43534</v>
       </c>
       <c r="D11" s="3">
-        <v>34396</v>
+        <v>35897</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="3">
-        <v>34396</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17949</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2019</v>
       </c>
@@ -679,19 +678,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="4">
-        <v>43507</v>
+        <v>43535</v>
       </c>
       <c r="D12" s="3">
-        <v>96536</v>
+        <v>367798</v>
       </c>
       <c r="E12" s="2">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F12" s="3">
-        <v>12067</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2019</v>
       </c>
@@ -699,19 +698,19 @@
         <v>6</v>
       </c>
       <c r="C13" s="4">
-        <v>43508</v>
+        <v>43536</v>
       </c>
       <c r="D13" s="3">
-        <v>234247</v>
+        <v>261702</v>
       </c>
       <c r="E13" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F13" s="3">
-        <v>15616</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13085</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2019</v>
       </c>
@@ -719,276 +718,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="4">
-        <v>43509</v>
+        <v>43537</v>
       </c>
       <c r="D14" s="3">
-        <v>78866</v>
+        <v>234163</v>
       </c>
       <c r="E14" s="2">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3">
-        <v>13144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4">
-        <v>43510</v>
-      </c>
-      <c r="D15" s="3">
-        <v>215446</v>
-      </c>
-      <c r="E15" s="2">
-        <v>15</v>
-      </c>
-      <c r="F15" s="3">
-        <v>14363</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4">
-        <v>43511</v>
-      </c>
-      <c r="D16" s="3">
-        <v>261167</v>
-      </c>
-      <c r="E16" s="2">
-        <v>20</v>
-      </c>
-      <c r="F16" s="3">
-        <v>13058</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4">
-        <v>43512</v>
-      </c>
-      <c r="D17" s="3">
-        <v>69495</v>
-      </c>
-      <c r="E17" s="2">
-        <v>6</v>
-      </c>
-      <c r="F17" s="3">
-        <v>11583</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4">
-        <v>43513</v>
-      </c>
-      <c r="D18" s="3">
-        <v>78074</v>
-      </c>
-      <c r="E18" s="2">
-        <v>4</v>
-      </c>
-      <c r="F18" s="3">
-        <v>19519</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4">
-        <v>43514</v>
-      </c>
-      <c r="D19" s="3">
-        <v>93626</v>
-      </c>
-      <c r="E19" s="2">
-        <v>10</v>
-      </c>
-      <c r="F19" s="3">
-        <v>9363</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="4">
-        <v>43515</v>
-      </c>
-      <c r="D20" s="3">
-        <v>213224</v>
-      </c>
-      <c r="E20" s="2">
-        <v>16</v>
-      </c>
-      <c r="F20" s="3">
-        <v>13327</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4">
-        <v>43516</v>
-      </c>
-      <c r="D21" s="3">
-        <v>153105</v>
-      </c>
-      <c r="E21" s="2">
-        <v>16</v>
-      </c>
-      <c r="F21" s="3">
-        <v>9569</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4">
-        <v>43517</v>
-      </c>
-      <c r="D22" s="3">
-        <v>168489</v>
-      </c>
-      <c r="E22" s="2">
-        <v>17</v>
-      </c>
-      <c r="F22" s="3">
-        <v>9911</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="4">
-        <v>43518</v>
-      </c>
-      <c r="D23" s="3">
-        <v>134792</v>
-      </c>
-      <c r="E23" s="2">
-        <v>13</v>
-      </c>
-      <c r="F23" s="3">
-        <v>10369</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="4">
-        <v>43519</v>
-      </c>
-      <c r="D24" s="3">
-        <v>108725</v>
-      </c>
-      <c r="E24" s="2">
-        <v>9</v>
-      </c>
-      <c r="F24" s="3">
-        <v>12081</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="4">
-        <v>43520</v>
-      </c>
-      <c r="D25" s="3">
-        <v>58396</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4</v>
-      </c>
-      <c r="F25" s="3">
-        <v>14599</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>2019</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="4">
-        <v>43521</v>
-      </c>
-      <c r="D26" s="3">
-        <v>327179</v>
-      </c>
-      <c r="E26" s="2">
-        <v>24</v>
-      </c>
-      <c r="F26" s="3">
-        <v>13632</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="4">
-        <v>43522</v>
-      </c>
-      <c r="D27" s="7">
-        <v>210000</v>
-      </c>
-      <c r="E27" s="8">
-        <v>17</v>
-      </c>
-      <c r="F27" s="7">
-        <v>12352.9411764706</v>
+        <v>12324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Innitiating Occupancy Forecast by Extracting Data And Creating New Folder
</commit_message>
<xml_diff>
--- a/PDN/data.xlsx
+++ b/PDN/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexisalvarez\OneDrive - Grupo Vidanta\UPDATE\Work\01. 26Dic18 - Metas PowerBI\Enero2019\_Forecast\GoalsForecastsAndProbabilites\PDN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="6_{74FE8280-A592-4FC4-BF0E-F114E96E327C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5D35CFE9-BC32-4677-B4B4-59A549289810}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="6_{74FE8280-A592-4FC4-BF0E-F114E96E327C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{AF3CB8F5-67F2-4C5E-A4EB-EBC24C1223D4}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="0" windowWidth="9030" windowHeight="2480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8720" yWindow="0" windowWidth="9030" windowHeight="2480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
   <si>
     <t>Año</t>
   </si>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F20">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mes"/>
@@ -439,11 +439,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -481,13 +479,13 @@
         <v>43525</v>
       </c>
       <c r="D2" s="3">
-        <v>204889</v>
+        <v>187889</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>20489</v>
+        <v>20877</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -561,13 +559,13 @@
         <v>43529</v>
       </c>
       <c r="D6" s="3">
-        <v>304511</v>
+        <v>265513</v>
       </c>
       <c r="E6" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3">
-        <v>17912</v>
+        <v>17701</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -641,13 +639,13 @@
         <v>43533</v>
       </c>
       <c r="D10" s="3">
-        <v>259888</v>
+        <v>205890</v>
       </c>
       <c r="E10" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3">
-        <v>14438</v>
+        <v>12868</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -728,6 +726,126 @@
       </c>
       <c r="F14" s="3">
         <v>12324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43538</v>
+      </c>
+      <c r="D15" s="3">
+        <v>456763</v>
+      </c>
+      <c r="E15" s="2">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3">
+        <v>21751</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4">
+        <v>43539</v>
+      </c>
+      <c r="D16" s="3">
+        <v>434511</v>
+      </c>
+      <c r="E16" s="2">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3">
+        <v>21726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4">
+        <v>43540</v>
+      </c>
+      <c r="D17" s="3">
+        <v>124044</v>
+      </c>
+      <c r="E17" s="2">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3">
+        <v>13783</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4">
+        <v>43541</v>
+      </c>
+      <c r="D18" s="3">
+        <v>19498</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>9749</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4">
+        <v>43542</v>
+      </c>
+      <c r="D19" s="3">
+        <v>210018</v>
+      </c>
+      <c r="E19" s="2">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3">
+        <v>15001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4">
+        <v>43543</v>
+      </c>
+      <c r="D20" s="3">
+        <v>153867</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3">
+        <v>15387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Provisional Occupancy Forecast
</commit_message>
<xml_diff>
--- a/PDN/data.xlsx
+++ b/PDN/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexisalvarez\OneDrive - Grupo Vidanta\UPDATE\Work\01. 26Dic18 - Metas PowerBI\Enero2019\_Forecast\GoalsForecastsAndProbabilites\PDN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="6_{74FE8280-A592-4FC4-BF0E-F114E96E327C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{AF3CB8F5-67F2-4C5E-A4EB-EBC24C1223D4}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="6_{74FE8280-A592-4FC4-BF0E-F114E96E327C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0BF10E9D-16A0-4001-A235-820D4D7D8AA8}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="0" windowWidth="9030" windowHeight="2480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="0" windowWidth="9030" windowHeight="2480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
   <si>
     <t>Año</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>Producción</t>
-  </si>
-  <si>
-    <t>#Reservas</t>
-  </si>
-  <si>
-    <t>I.P.P.R.</t>
   </si>
   <si>
     <t>marzo</t>
@@ -89,23 +83,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="164" formatCode="\$#,##0;\(\$#,##0\);\$#,##0"/>
     </dxf>
@@ -129,14 +116,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F20">
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D21">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fechaa" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Producción" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="#Reservas" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="I.P.P.R." dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fechaa" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Producción" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -439,16 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,391 +446,285 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2019</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3">
         <v>43525</v>
       </c>
-      <c r="D2" s="3">
-        <v>187889</v>
-      </c>
-      <c r="E2" s="2">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3">
-        <v>20877</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D2" s="2">
+        <v>125112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
         <v>43526</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>34996</v>
       </c>
-      <c r="E3" s="2">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3">
-        <v>6999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2019</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
         <v>43527</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>51399</v>
       </c>
-      <c r="E4" s="2">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3">
-        <v>12850</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2019</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
         <v>43528</v>
       </c>
-      <c r="D5" s="3">
-        <v>252847</v>
-      </c>
-      <c r="E5" s="2">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3">
-        <v>22986</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D5" s="2">
+        <v>247847</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2019</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
         <v>43529</v>
       </c>
-      <c r="D6" s="3">
-        <v>265513</v>
-      </c>
-      <c r="E6" s="2">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3">
-        <v>17701</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D6" s="2">
+        <v>313151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2019</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
         <v>43530</v>
       </c>
-      <c r="D7" s="3">
-        <v>283817</v>
-      </c>
-      <c r="E7" s="2">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3">
-        <v>18921</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D7" s="2">
+        <v>289816</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2019</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
         <v>43531</v>
       </c>
-      <c r="D8" s="3">
-        <v>167152</v>
-      </c>
-      <c r="E8" s="2">
-        <v>13</v>
-      </c>
-      <c r="F8" s="3">
-        <v>12858</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D8" s="2">
+        <v>275392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2019</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
         <v>43532</v>
       </c>
-      <c r="D9" s="3">
-        <v>445397</v>
-      </c>
-      <c r="E9" s="2">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3">
-        <v>29693</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D9" s="2">
+        <v>355071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2019</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
         <v>43533</v>
       </c>
-      <c r="D10" s="3">
-        <v>205890</v>
-      </c>
-      <c r="E10" s="2">
-        <v>16</v>
-      </c>
-      <c r="F10" s="3">
-        <v>12868</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D10" s="2">
+        <v>315789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2019</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
         <v>43534</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>35897</v>
       </c>
-      <c r="E11" s="2">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3">
-        <v>17949</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2019</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
         <v>43535</v>
       </c>
-      <c r="D12" s="3">
-        <v>367798</v>
-      </c>
-      <c r="E12" s="2">
-        <v>18</v>
-      </c>
-      <c r="F12" s="3">
-        <v>20433</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D12" s="2">
+        <v>314798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2019</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
         <v>43536</v>
       </c>
-      <c r="D13" s="3">
-        <v>261702</v>
-      </c>
-      <c r="E13" s="2">
-        <v>20</v>
-      </c>
-      <c r="F13" s="3">
-        <v>13085</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D13" s="2">
+        <v>263702</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2019</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
         <v>43537</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>234163</v>
       </c>
-      <c r="E14" s="2">
-        <v>19</v>
-      </c>
-      <c r="F14" s="3">
-        <v>12324</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2019</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
         <v>43538</v>
       </c>
-      <c r="D15" s="3">
-        <v>456763</v>
-      </c>
-      <c r="E15" s="2">
-        <v>21</v>
-      </c>
-      <c r="F15" s="3">
-        <v>21751</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D15" s="2">
+        <v>406265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2019</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3">
         <v>43539</v>
       </c>
-      <c r="D16" s="3">
-        <v>434511</v>
-      </c>
-      <c r="E16" s="2">
-        <v>20</v>
-      </c>
-      <c r="F16" s="3">
-        <v>21726</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D16" s="2">
+        <v>436279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2019</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
         <v>43540</v>
       </c>
-      <c r="D17" s="3">
-        <v>124044</v>
-      </c>
-      <c r="E17" s="2">
-        <v>9</v>
-      </c>
-      <c r="F17" s="3">
-        <v>13783</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D17" s="2">
+        <v>123544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2019</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3">
         <v>43541</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>19498</v>
       </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3">
-        <v>9749</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2019</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3">
         <v>43542</v>
       </c>
-      <c r="D19" s="3">
-        <v>210018</v>
-      </c>
-      <c r="E19" s="2">
-        <v>14</v>
-      </c>
-      <c r="F19" s="3">
-        <v>15001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D19" s="2">
+        <v>211018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2019</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3">
         <v>43543</v>
       </c>
-      <c r="D20" s="3">
-        <v>153867</v>
-      </c>
-      <c r="E20" s="2">
-        <v>10</v>
-      </c>
-      <c r="F20" s="3">
-        <v>15387</v>
+      <c r="D20" s="2">
+        <v>116869</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3">
+        <v>43544</v>
+      </c>
+      <c r="D21" s="2">
+        <v>279364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>